<commit_message>
Averaged Data Table created
</commit_message>
<xml_diff>
--- a/Research Corpus/Data by Source/Source_10~Cloud-Edge-End Collaborative Computing-Enabled Intelligent Sharding Blockchain for Industrial IoT Based on PPO Approach.xlsx
+++ b/Research Corpus/Data by Source/Source_10~Cloud-Edge-End Collaborative Computing-Enabled Intelligent Sharding Blockchain for Industrial IoT Based on PPO Approach.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yawu/Desktop/Repos/FT324_SLR/Research Corpus/Data by Source/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\FT324_SLR\Research Corpus\Data by Source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA3F7A23-4851-594B-AFB8-1317A9302A29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{894A2AED-2B08-430E-8F55-AE8209E5992C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="1000" windowWidth="27640" windowHeight="15880" xr2:uid="{754419C1-0F3F-3647-A532-9827BA1C8B7E}"/>
+    <workbookView xWindow="-28920" yWindow="2715" windowWidth="29040" windowHeight="15720" xr2:uid="{754419C1-0F3F-3647-A532-9827BA1C8B7E}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -133,20 +133,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="6">
     <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
       <font>
@@ -166,6 +172,15 @@
         <scheme val="minor"/>
       </font>
     </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -184,11 +199,11 @@
   <autoFilter ref="A1:G10" xr:uid="{115EDC2F-E161-E541-948B-57B318B7A756}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{24CAED38-1FCD-B84A-9A81-286811F58FD3}" name="Consensus"/>
-    <tableColumn id="2" xr3:uid="{1FC090FA-D53D-9945-9980-31B77B7C1A40}" name="TPS"/>
-    <tableColumn id="3" xr3:uid="{0CF134D6-57BB-DE46-84F0-9B00275184E1}" name="Energy Use per Transaction"/>
-    <tableColumn id="4" xr3:uid="{C183822B-94EB-194A-80D3-7FD19859150F}" name="Nakamoto Coefficient"/>
-    <tableColumn id="5" xr3:uid="{2B11CD8D-8F08-3C4D-A40A-DE6AAEB5FE56}" name="% of nodes required to take over network" dataDxfId="1" dataCellStyle="Percent"/>
-    <tableColumn id="6" xr3:uid="{3AE017AC-E138-5C46-9867-98FB57A97641}" name="Strengths"/>
+    <tableColumn id="2" xr3:uid="{1FC090FA-D53D-9945-9980-31B77B7C1A40}" name="TPS" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{0CF134D6-57BB-DE46-84F0-9B00275184E1}" name="Energy Use per Transaction" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{C183822B-94EB-194A-80D3-7FD19859150F}" name="Nakamoto Coefficient" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{2B11CD8D-8F08-3C4D-A40A-DE6AAEB5FE56}" name="% of nodes required to take over network" dataDxfId="2" dataCellStyle="Percent"/>
+    <tableColumn id="6" xr3:uid="{3AE017AC-E138-5C46-9867-98FB57A97641}" name="Strengths" dataDxfId="1"/>
     <tableColumn id="7" xr3:uid="{0A1B6FA4-07C8-3149-B875-83ABDFEE8046}" name="Weaknesses" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -515,21 +530,21 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.33203125" customWidth="1"/>
+    <col min="1" max="1" width="37.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.375" customWidth="1"/>
     <col min="3" max="3" width="25" customWidth="1"/>
-    <col min="4" max="4" width="21.1640625" customWidth="1"/>
-    <col min="5" max="5" width="35.6640625" customWidth="1"/>
-    <col min="6" max="6" width="11.1640625" customWidth="1"/>
+    <col min="4" max="4" width="21.125" customWidth="1"/>
+    <col min="5" max="5" width="35.625" customWidth="1"/>
+    <col min="6" max="6" width="11.125" customWidth="1"/>
     <col min="7" max="7" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -552,210 +567,210 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="B2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="B3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="B4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
-      <c r="B5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="B5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
-      <c r="B6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" t="s">
-        <v>16</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="B6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
-      <c r="B7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7" t="s">
-        <v>16</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="B7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
-      <c r="B8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8" t="s">
-        <v>16</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="170" x14ac:dyDescent="0.2">
+      <c r="B8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="157.5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
-      <c r="B9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F9" t="s">
-        <v>16</v>
-      </c>
-      <c r="G9" s="1" t="s">
+      <c r="B9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>15</v>
       </c>
-      <c r="B10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F10" t="s">
-        <v>16</v>
-      </c>
-      <c r="G10" s="1" t="s">
+      <c r="B10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" s="4" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>